<commit_message>
Updated predator-prey interaction summaries and scripts for lake BT
</commit_message>
<xml_diff>
--- a/data/encounters/pike_deaths.xlsx
+++ b/data/encounters/pike_deaths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcusMichelangeli\GIT projects\Git_repo\drugged_lakes_griffith_repo\drugged_lakes\data\encounters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F196E4E-2185-4A01-92EF-BFE1008D034D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C53230A-8F89-46FB-9AD5-A897C2C918A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2385" windowWidth="26415" windowHeight="7845" xr2:uid="{9810EA30-B907-4C4B-B0F0-066916FA9DE2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9810EA30-B907-4C4B-B0F0-066916FA9DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>44841</v>
+        <v>44830</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>44848</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>